<commit_message>
add paper template, FIPS code to data, data dictionary
</commit_message>
<xml_diff>
--- a/reference/20220805 Data Dictionary.xlsx
+++ b/reference/20220805 Data Dictionary.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Datasets" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="County Area Infrastructure Spen" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,18 +21,115 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+  <si>
+    <t xml:space="preserve">Dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">County Area Expenditures A (1957-2002).Rds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local government expenditures aggregated at the county level at five year intervals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See workbook “.../data/Historical_Finance_Data/County_Area_Fin/_Finance_Publication_Data_Guide.xls”, tabs 5a and 5b for field definitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022072 Import ASSLGF Data (Historical)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">County Area Expenditures B (1957-2002).Rds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">County Area Expenditures Revenues (1957-2002).Rds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local government revenues aggregated at the county level at five year intervals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">County Area Infrastructure Spending (1957 - 2002).Rds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inflation-adjusted direct expenditures on highways and sewerage by county at five year intervals.</t>
+  </si>
   <si>
     <t xml:space="preserve">Field</t>
   </si>
   <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
     <t xml:space="preserve">Source</t>
   </si>
   <si>
-    <t xml:space="preserve">Link</t>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey year, which includes each individual government fiscal year that ended between July 1 of the previous
+year and June 30 of the survey year. See 2006 Classification Manual for details.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Census</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOVS ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIPS.Code.State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIPS.Code.County</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPI for All Urban Consumers (CPI-U)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular.Hwy.Cur.Oper..E44.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular.Hwy.Direct.Exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular.Hwy.Cap.Outlay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sewerage.Current.Oper..E80.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sewerage.Direct.Expend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sewerage.Cap.Outlay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW.Mgmt.Current.Oper..E81.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW.Mgmt.Direct.Expend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW.Mgmt.Capital.Outlay</t>
   </si>
 </sst>
 </file>
@@ -113,13 +211,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -139,47 +241,236 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="71.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="85.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="11.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
standardize ASSLGF data to long format with finance codes
</commit_message>
<xml_diff>
--- a/reference/20220805 Data Dictionary.xlsx
+++ b/reference/20220805 Data Dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t xml:space="preserve">Dataset</t>
   </si>
@@ -38,10 +38,10 @@
     <t xml:space="preserve">Link</t>
   </si>
   <si>
-    <t xml:space="preserve">County Area Expenditures A (1957-2002).Rds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Local government expenditures aggregated at the county level at five year intervals.</t>
+    <t xml:space="preserve">County Area Finances (1957-2002).Rds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local government revenues expenditures aggregated at the county level at five year intervals.</t>
   </si>
   <si>
     <t xml:space="preserve">See workbook “.../data/Historical_Finance_Data/County_Area_Fin/_Finance_Publication_Data_Guide.xls”, tabs 5a and 5b for field definitions</t>
@@ -50,19 +50,19 @@
     <t xml:space="preserve">2022072 Import ASSLGF Data (Historical)</t>
   </si>
   <si>
-    <t xml:space="preserve">County Area Expenditures B (1957-2002).Rds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">County Area Expenditures Revenues (1957-2002).Rds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Local government revenues aggregated at the county level at five year intervals.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">County Area Infrastructure Spending (1957 - 2002).Rds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inflation-adjusted direct expenditures on highways and sewerage by county at five year intervals.</t>
+    <t xml:space="preserve">County Area Population (1957-2002).Rds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population by county along with county name and FIPS code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">County Area Finances (2007-2012).Rds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local government revenues and expenditures for 2007 and 2012.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See “.../data/Historical_Finance_Data/County_Area_Finances_YEAR” for information on 2007 and 2012 data</t>
   </si>
   <si>
     <t xml:space="preserve">Field</t>
@@ -211,7 +211,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,6 +222,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -241,12 +245,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -294,10 +298,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -305,33 +306,1048 @@
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="O5" s="0"/>
+      <c r="P5" s="0"/>
+      <c r="Q5" s="0"/>
+      <c r="R5" s="0"/>
+      <c r="S5" s="0"/>
+      <c r="T5" s="0"/>
+      <c r="U5" s="0"/>
+      <c r="V5" s="0"/>
+      <c r="W5" s="0"/>
+      <c r="X5" s="0"/>
+      <c r="Y5" s="0"/>
+      <c r="Z5" s="0"/>
+      <c r="AA5" s="0"/>
+      <c r="AB5" s="0"/>
+      <c r="AC5" s="0"/>
+      <c r="AD5" s="0"/>
+      <c r="AE5" s="0"/>
+      <c r="AF5" s="0"/>
+      <c r="AG5" s="0"/>
+      <c r="AH5" s="0"/>
+      <c r="AI5" s="0"/>
+      <c r="AJ5" s="0"/>
+      <c r="AK5" s="0"/>
+      <c r="AL5" s="0"/>
+      <c r="AM5" s="0"/>
+      <c r="AN5" s="0"/>
+      <c r="AO5" s="0"/>
+      <c r="AP5" s="0"/>
+      <c r="AQ5" s="0"/>
+      <c r="AR5" s="0"/>
+      <c r="AS5" s="0"/>
+      <c r="AT5" s="0"/>
+      <c r="AU5" s="0"/>
+      <c r="AV5" s="0"/>
+      <c r="AW5" s="0"/>
+      <c r="AX5" s="0"/>
+      <c r="AY5" s="0"/>
+      <c r="AZ5" s="0"/>
+      <c r="BA5" s="0"/>
+      <c r="BB5" s="0"/>
+      <c r="BC5" s="0"/>
+      <c r="BD5" s="0"/>
+      <c r="BE5" s="0"/>
+      <c r="BF5" s="0"/>
+      <c r="BG5" s="0"/>
+      <c r="BH5" s="0"/>
+      <c r="BI5" s="0"/>
+      <c r="BJ5" s="0"/>
+      <c r="BK5" s="0"/>
+      <c r="BL5" s="0"/>
+      <c r="BM5" s="0"/>
+      <c r="BN5" s="0"/>
+      <c r="BO5" s="0"/>
+      <c r="BP5" s="0"/>
+      <c r="BQ5" s="0"/>
+      <c r="BR5" s="0"/>
+      <c r="BS5" s="0"/>
+      <c r="BT5" s="0"/>
+      <c r="BU5" s="0"/>
+      <c r="BV5" s="0"/>
+      <c r="BW5" s="0"/>
+      <c r="BX5" s="0"/>
+      <c r="BY5" s="0"/>
+      <c r="BZ5" s="0"/>
+      <c r="CA5" s="0"/>
+      <c r="CB5" s="0"/>
+      <c r="CC5" s="0"/>
+      <c r="CD5" s="0"/>
+      <c r="CE5" s="0"/>
+      <c r="CF5" s="0"/>
+      <c r="CG5" s="0"/>
+      <c r="CH5" s="0"/>
+      <c r="CI5" s="0"/>
+      <c r="CJ5" s="0"/>
+      <c r="CK5" s="0"/>
+      <c r="CL5" s="0"/>
+      <c r="CM5" s="0"/>
+      <c r="CN5" s="0"/>
+      <c r="CO5" s="0"/>
+      <c r="CP5" s="0"/>
+      <c r="CQ5" s="0"/>
+      <c r="CR5" s="0"/>
+      <c r="CS5" s="0"/>
+      <c r="CT5" s="0"/>
+      <c r="CU5" s="0"/>
+      <c r="CV5" s="0"/>
+      <c r="CW5" s="0"/>
+      <c r="CX5" s="0"/>
+      <c r="CY5" s="0"/>
+      <c r="CZ5" s="0"/>
+      <c r="DA5" s="0"/>
+      <c r="DB5" s="0"/>
+      <c r="DC5" s="0"/>
+      <c r="DD5" s="0"/>
+      <c r="DE5" s="0"/>
+      <c r="DF5" s="0"/>
+      <c r="DG5" s="0"/>
+      <c r="DH5" s="0"/>
+      <c r="DI5" s="0"/>
+      <c r="DJ5" s="0"/>
+      <c r="DK5" s="0"/>
+      <c r="DL5" s="0"/>
+      <c r="DM5" s="0"/>
+      <c r="DN5" s="0"/>
+      <c r="DO5" s="0"/>
+      <c r="DP5" s="0"/>
+      <c r="DQ5" s="0"/>
+      <c r="DR5" s="0"/>
+      <c r="DS5" s="0"/>
+      <c r="DT5" s="0"/>
+      <c r="DU5" s="0"/>
+      <c r="DV5" s="0"/>
+      <c r="DW5" s="0"/>
+      <c r="DX5" s="0"/>
+      <c r="DY5" s="0"/>
+      <c r="DZ5" s="0"/>
+      <c r="EA5" s="0"/>
+      <c r="EB5" s="0"/>
+      <c r="EC5" s="0"/>
+      <c r="ED5" s="0"/>
+      <c r="EE5" s="0"/>
+      <c r="EF5" s="0"/>
+      <c r="EG5" s="0"/>
+      <c r="EH5" s="0"/>
+      <c r="EI5" s="0"/>
+      <c r="EJ5" s="0"/>
+      <c r="EK5" s="0"/>
+      <c r="EL5" s="0"/>
+      <c r="EM5" s="0"/>
+      <c r="EN5" s="0"/>
+      <c r="EO5" s="0"/>
+      <c r="EP5" s="0"/>
+      <c r="EQ5" s="0"/>
+      <c r="ER5" s="0"/>
+      <c r="ES5" s="0"/>
+      <c r="ET5" s="0"/>
+      <c r="EU5" s="0"/>
+      <c r="EV5" s="0"/>
+      <c r="EW5" s="0"/>
+      <c r="EX5" s="0"/>
+      <c r="EY5" s="0"/>
+      <c r="EZ5" s="0"/>
+      <c r="FA5" s="0"/>
+      <c r="FB5" s="0"/>
+      <c r="FC5" s="0"/>
+      <c r="FD5" s="0"/>
+      <c r="FE5" s="0"/>
+      <c r="FF5" s="0"/>
+      <c r="FG5" s="0"/>
+      <c r="FH5" s="0"/>
+      <c r="FI5" s="0"/>
+      <c r="FJ5" s="0"/>
+      <c r="FK5" s="0"/>
+      <c r="FL5" s="0"/>
+      <c r="FM5" s="0"/>
+      <c r="FN5" s="0"/>
+      <c r="FO5" s="0"/>
+      <c r="FP5" s="0"/>
+      <c r="FQ5" s="0"/>
+      <c r="FR5" s="0"/>
+      <c r="FS5" s="0"/>
+      <c r="FT5" s="0"/>
+      <c r="FU5" s="0"/>
+      <c r="FV5" s="0"/>
+      <c r="FW5" s="0"/>
+      <c r="FX5" s="0"/>
+      <c r="FY5" s="0"/>
+      <c r="FZ5" s="0"/>
+      <c r="GA5" s="0"/>
+      <c r="GB5" s="0"/>
+      <c r="GC5" s="0"/>
+      <c r="GD5" s="0"/>
+      <c r="GE5" s="0"/>
+      <c r="GF5" s="0"/>
+      <c r="GG5" s="0"/>
+      <c r="GH5" s="0"/>
+      <c r="GI5" s="0"/>
+      <c r="GJ5" s="0"/>
+      <c r="GK5" s="0"/>
+      <c r="GL5" s="0"/>
+      <c r="GM5" s="0"/>
+      <c r="GN5" s="0"/>
+      <c r="GO5" s="0"/>
+      <c r="GP5" s="0"/>
+      <c r="GQ5" s="0"/>
+      <c r="GR5" s="0"/>
+      <c r="GS5" s="0"/>
+      <c r="GT5" s="0"/>
+      <c r="GU5" s="0"/>
+      <c r="GV5" s="0"/>
+      <c r="GW5" s="0"/>
+      <c r="GX5" s="0"/>
+      <c r="GY5" s="0"/>
+      <c r="GZ5" s="0"/>
+      <c r="HA5" s="0"/>
+      <c r="HB5" s="0"/>
+      <c r="HC5" s="0"/>
+      <c r="HD5" s="0"/>
+      <c r="HE5" s="0"/>
+      <c r="HF5" s="0"/>
+      <c r="HG5" s="0"/>
+      <c r="HH5" s="0"/>
+      <c r="HI5" s="0"/>
+      <c r="HJ5" s="0"/>
+      <c r="HK5" s="0"/>
+      <c r="HL5" s="0"/>
+      <c r="HM5" s="0"/>
+      <c r="HN5" s="0"/>
+      <c r="HO5" s="0"/>
+      <c r="HP5" s="0"/>
+      <c r="HQ5" s="0"/>
+      <c r="HR5" s="0"/>
+      <c r="HS5" s="0"/>
+      <c r="HT5" s="0"/>
+      <c r="HU5" s="0"/>
+      <c r="HV5" s="0"/>
+      <c r="HW5" s="0"/>
+      <c r="HX5" s="0"/>
+      <c r="HY5" s="0"/>
+      <c r="HZ5" s="0"/>
+      <c r="IA5" s="0"/>
+      <c r="IB5" s="0"/>
+      <c r="IC5" s="0"/>
+      <c r="ID5" s="0"/>
+      <c r="IE5" s="0"/>
+      <c r="IF5" s="0"/>
+      <c r="IG5" s="0"/>
+      <c r="IH5" s="0"/>
+      <c r="II5" s="0"/>
+      <c r="IJ5" s="0"/>
+      <c r="IK5" s="0"/>
+      <c r="IL5" s="0"/>
+      <c r="IM5" s="0"/>
+      <c r="IN5" s="0"/>
+      <c r="IO5" s="0"/>
+      <c r="IP5" s="0"/>
+      <c r="IQ5" s="0"/>
+      <c r="IR5" s="0"/>
+      <c r="IS5" s="0"/>
+      <c r="IT5" s="0"/>
+      <c r="IU5" s="0"/>
+      <c r="IV5" s="0"/>
+      <c r="IW5" s="0"/>
+      <c r="IX5" s="0"/>
+      <c r="IY5" s="0"/>
+      <c r="IZ5" s="0"/>
+      <c r="JA5" s="0"/>
+      <c r="JB5" s="0"/>
+      <c r="JC5" s="0"/>
+      <c r="JD5" s="0"/>
+      <c r="JE5" s="0"/>
+      <c r="JF5" s="0"/>
+      <c r="JG5" s="0"/>
+      <c r="JH5" s="0"/>
+      <c r="JI5" s="0"/>
+      <c r="JJ5" s="0"/>
+      <c r="JK5" s="0"/>
+      <c r="JL5" s="0"/>
+      <c r="JM5" s="0"/>
+      <c r="JN5" s="0"/>
+      <c r="JO5" s="0"/>
+      <c r="JP5" s="0"/>
+      <c r="JQ5" s="0"/>
+      <c r="JR5" s="0"/>
+      <c r="JS5" s="0"/>
+      <c r="JT5" s="0"/>
+      <c r="JU5" s="0"/>
+      <c r="JV5" s="0"/>
+      <c r="JW5" s="0"/>
+      <c r="JX5" s="0"/>
+      <c r="JY5" s="0"/>
+      <c r="JZ5" s="0"/>
+      <c r="KA5" s="0"/>
+      <c r="KB5" s="0"/>
+      <c r="KC5" s="0"/>
+      <c r="KD5" s="0"/>
+      <c r="KE5" s="0"/>
+      <c r="KF5" s="0"/>
+      <c r="KG5" s="0"/>
+      <c r="KH5" s="0"/>
+      <c r="KI5" s="0"/>
+      <c r="KJ5" s="0"/>
+      <c r="KK5" s="0"/>
+      <c r="KL5" s="0"/>
+      <c r="KM5" s="0"/>
+      <c r="KN5" s="0"/>
+      <c r="KO5" s="0"/>
+      <c r="KP5" s="0"/>
+      <c r="KQ5" s="0"/>
+      <c r="KR5" s="0"/>
+      <c r="KS5" s="0"/>
+      <c r="KT5" s="0"/>
+      <c r="KU5" s="0"/>
+      <c r="KV5" s="0"/>
+      <c r="KW5" s="0"/>
+      <c r="KX5" s="0"/>
+      <c r="KY5" s="0"/>
+      <c r="KZ5" s="0"/>
+      <c r="LA5" s="0"/>
+      <c r="LB5" s="0"/>
+      <c r="LC5" s="0"/>
+      <c r="LD5" s="0"/>
+      <c r="LE5" s="0"/>
+      <c r="LF5" s="0"/>
+      <c r="LG5" s="0"/>
+      <c r="LH5" s="0"/>
+      <c r="LI5" s="0"/>
+      <c r="LJ5" s="0"/>
+      <c r="LK5" s="0"/>
+      <c r="LL5" s="0"/>
+      <c r="LM5" s="0"/>
+      <c r="LN5" s="0"/>
+      <c r="LO5" s="0"/>
+      <c r="LP5" s="0"/>
+      <c r="LQ5" s="0"/>
+      <c r="LR5" s="0"/>
+      <c r="LS5" s="0"/>
+      <c r="LT5" s="0"/>
+      <c r="LU5" s="0"/>
+      <c r="LV5" s="0"/>
+      <c r="LW5" s="0"/>
+      <c r="LX5" s="0"/>
+      <c r="LY5" s="0"/>
+      <c r="LZ5" s="0"/>
+      <c r="MA5" s="0"/>
+      <c r="MB5" s="0"/>
+      <c r="MC5" s="0"/>
+      <c r="MD5" s="0"/>
+      <c r="ME5" s="0"/>
+      <c r="MF5" s="0"/>
+      <c r="MG5" s="0"/>
+      <c r="MH5" s="0"/>
+      <c r="MI5" s="0"/>
+      <c r="MJ5" s="0"/>
+      <c r="MK5" s="0"/>
+      <c r="ML5" s="0"/>
+      <c r="MM5" s="0"/>
+      <c r="MN5" s="0"/>
+      <c r="MO5" s="0"/>
+      <c r="MP5" s="0"/>
+      <c r="MQ5" s="0"/>
+      <c r="MR5" s="0"/>
+      <c r="MS5" s="0"/>
+      <c r="MT5" s="0"/>
+      <c r="MU5" s="0"/>
+      <c r="MV5" s="0"/>
+      <c r="MW5" s="0"/>
+      <c r="MX5" s="0"/>
+      <c r="MY5" s="0"/>
+      <c r="MZ5" s="0"/>
+      <c r="NA5" s="0"/>
+      <c r="NB5" s="0"/>
+      <c r="NC5" s="0"/>
+      <c r="ND5" s="0"/>
+      <c r="NE5" s="0"/>
+      <c r="NF5" s="0"/>
+      <c r="NG5" s="0"/>
+      <c r="NH5" s="0"/>
+      <c r="NI5" s="0"/>
+      <c r="NJ5" s="0"/>
+      <c r="NK5" s="0"/>
+      <c r="NL5" s="0"/>
+      <c r="NM5" s="0"/>
+      <c r="NN5" s="0"/>
+      <c r="NO5" s="0"/>
+      <c r="NP5" s="0"/>
+      <c r="NQ5" s="0"/>
+      <c r="NR5" s="0"/>
+      <c r="NS5" s="0"/>
+      <c r="NT5" s="0"/>
+      <c r="NU5" s="0"/>
+      <c r="NV5" s="0"/>
+      <c r="NW5" s="0"/>
+      <c r="NX5" s="0"/>
+      <c r="NY5" s="0"/>
+      <c r="NZ5" s="0"/>
+      <c r="OA5" s="0"/>
+      <c r="OB5" s="0"/>
+      <c r="OC5" s="0"/>
+      <c r="OD5" s="0"/>
+      <c r="OE5" s="0"/>
+      <c r="OF5" s="0"/>
+      <c r="OG5" s="0"/>
+      <c r="OH5" s="0"/>
+      <c r="OI5" s="0"/>
+      <c r="OJ5" s="0"/>
+      <c r="OK5" s="0"/>
+      <c r="OL5" s="0"/>
+      <c r="OM5" s="0"/>
+      <c r="ON5" s="0"/>
+      <c r="OO5" s="0"/>
+      <c r="OP5" s="0"/>
+      <c r="OQ5" s="0"/>
+      <c r="OR5" s="0"/>
+      <c r="OS5" s="0"/>
+      <c r="OT5" s="0"/>
+      <c r="OU5" s="0"/>
+      <c r="OV5" s="0"/>
+      <c r="OW5" s="0"/>
+      <c r="OX5" s="0"/>
+      <c r="OY5" s="0"/>
+      <c r="OZ5" s="0"/>
+      <c r="PA5" s="0"/>
+      <c r="PB5" s="0"/>
+      <c r="PC5" s="0"/>
+      <c r="PD5" s="0"/>
+      <c r="PE5" s="0"/>
+      <c r="PF5" s="0"/>
+      <c r="PG5" s="0"/>
+      <c r="PH5" s="0"/>
+      <c r="PI5" s="0"/>
+      <c r="PJ5" s="0"/>
+      <c r="PK5" s="0"/>
+      <c r="PL5" s="0"/>
+      <c r="PM5" s="0"/>
+      <c r="PN5" s="0"/>
+      <c r="PO5" s="0"/>
+      <c r="PP5" s="0"/>
+      <c r="PQ5" s="0"/>
+      <c r="PR5" s="0"/>
+      <c r="PS5" s="0"/>
+      <c r="PT5" s="0"/>
+      <c r="PU5" s="0"/>
+      <c r="PV5" s="0"/>
+      <c r="PW5" s="0"/>
+      <c r="PX5" s="0"/>
+      <c r="PY5" s="0"/>
+      <c r="PZ5" s="0"/>
+      <c r="QA5" s="0"/>
+      <c r="QB5" s="0"/>
+      <c r="QC5" s="0"/>
+      <c r="QD5" s="0"/>
+      <c r="QE5" s="0"/>
+      <c r="QF5" s="0"/>
+      <c r="QG5" s="0"/>
+      <c r="QH5" s="0"/>
+      <c r="QI5" s="0"/>
+      <c r="QJ5" s="0"/>
+      <c r="QK5" s="0"/>
+      <c r="QL5" s="0"/>
+      <c r="QM5" s="0"/>
+      <c r="QN5" s="0"/>
+      <c r="QO5" s="0"/>
+      <c r="QP5" s="0"/>
+      <c r="QQ5" s="0"/>
+      <c r="QR5" s="0"/>
+      <c r="QS5" s="0"/>
+      <c r="QT5" s="0"/>
+      <c r="QU5" s="0"/>
+      <c r="QV5" s="0"/>
+      <c r="QW5" s="0"/>
+      <c r="QX5" s="0"/>
+      <c r="QY5" s="0"/>
+      <c r="QZ5" s="0"/>
+      <c r="RA5" s="0"/>
+      <c r="RB5" s="0"/>
+      <c r="RC5" s="0"/>
+      <c r="RD5" s="0"/>
+      <c r="RE5" s="0"/>
+      <c r="RF5" s="0"/>
+      <c r="RG5" s="0"/>
+      <c r="RH5" s="0"/>
+      <c r="RI5" s="0"/>
+      <c r="RJ5" s="0"/>
+      <c r="RK5" s="0"/>
+      <c r="RL5" s="0"/>
+      <c r="RM5" s="0"/>
+      <c r="RN5" s="0"/>
+      <c r="RO5" s="0"/>
+      <c r="RP5" s="0"/>
+      <c r="RQ5" s="0"/>
+      <c r="RR5" s="0"/>
+      <c r="RS5" s="0"/>
+      <c r="RT5" s="0"/>
+      <c r="RU5" s="0"/>
+      <c r="RV5" s="0"/>
+      <c r="RW5" s="0"/>
+      <c r="RX5" s="0"/>
+      <c r="RY5" s="0"/>
+      <c r="RZ5" s="0"/>
+      <c r="SA5" s="0"/>
+      <c r="SB5" s="0"/>
+      <c r="SC5" s="0"/>
+      <c r="SD5" s="0"/>
+      <c r="SE5" s="0"/>
+      <c r="SF5" s="0"/>
+      <c r="SG5" s="0"/>
+      <c r="SH5" s="0"/>
+      <c r="SI5" s="0"/>
+      <c r="SJ5" s="0"/>
+      <c r="SK5" s="0"/>
+      <c r="SL5" s="0"/>
+      <c r="SM5" s="0"/>
+      <c r="SN5" s="0"/>
+      <c r="SO5" s="0"/>
+      <c r="SP5" s="0"/>
+      <c r="SQ5" s="0"/>
+      <c r="SR5" s="0"/>
+      <c r="SS5" s="0"/>
+      <c r="ST5" s="0"/>
+      <c r="SU5" s="0"/>
+      <c r="SV5" s="0"/>
+      <c r="SW5" s="0"/>
+      <c r="SX5" s="0"/>
+      <c r="SY5" s="0"/>
+      <c r="SZ5" s="0"/>
+      <c r="TA5" s="0"/>
+      <c r="TB5" s="0"/>
+      <c r="TC5" s="0"/>
+      <c r="TD5" s="0"/>
+      <c r="TE5" s="0"/>
+      <c r="TF5" s="0"/>
+      <c r="TG5" s="0"/>
+      <c r="TH5" s="0"/>
+      <c r="TI5" s="0"/>
+      <c r="TJ5" s="0"/>
+      <c r="TK5" s="0"/>
+      <c r="TL5" s="0"/>
+      <c r="TM5" s="0"/>
+      <c r="TN5" s="0"/>
+      <c r="TO5" s="0"/>
+      <c r="TP5" s="0"/>
+      <c r="TQ5" s="0"/>
+      <c r="TR5" s="0"/>
+      <c r="TS5" s="0"/>
+      <c r="TT5" s="0"/>
+      <c r="TU5" s="0"/>
+      <c r="TV5" s="0"/>
+      <c r="TW5" s="0"/>
+      <c r="TX5" s="0"/>
+      <c r="TY5" s="0"/>
+      <c r="TZ5" s="0"/>
+      <c r="UA5" s="0"/>
+      <c r="UB5" s="0"/>
+      <c r="UC5" s="0"/>
+      <c r="UD5" s="0"/>
+      <c r="UE5" s="0"/>
+      <c r="UF5" s="0"/>
+      <c r="UG5" s="0"/>
+      <c r="UH5" s="0"/>
+      <c r="UI5" s="0"/>
+      <c r="UJ5" s="0"/>
+      <c r="UK5" s="0"/>
+      <c r="UL5" s="0"/>
+      <c r="UM5" s="0"/>
+      <c r="UN5" s="0"/>
+      <c r="UO5" s="0"/>
+      <c r="UP5" s="0"/>
+      <c r="UQ5" s="0"/>
+      <c r="UR5" s="0"/>
+      <c r="US5" s="0"/>
+      <c r="UT5" s="0"/>
+      <c r="UU5" s="0"/>
+      <c r="UV5" s="0"/>
+      <c r="UW5" s="0"/>
+      <c r="UX5" s="0"/>
+      <c r="UY5" s="0"/>
+      <c r="UZ5" s="0"/>
+      <c r="VA5" s="0"/>
+      <c r="VB5" s="0"/>
+      <c r="VC5" s="0"/>
+      <c r="VD5" s="0"/>
+      <c r="VE5" s="0"/>
+      <c r="VF5" s="0"/>
+      <c r="VG5" s="0"/>
+      <c r="VH5" s="0"/>
+      <c r="VI5" s="0"/>
+      <c r="VJ5" s="0"/>
+      <c r="VK5" s="0"/>
+      <c r="VL5" s="0"/>
+      <c r="VM5" s="0"/>
+      <c r="VN5" s="0"/>
+      <c r="VO5" s="0"/>
+      <c r="VP5" s="0"/>
+      <c r="VQ5" s="0"/>
+      <c r="VR5" s="0"/>
+      <c r="VS5" s="0"/>
+      <c r="VT5" s="0"/>
+      <c r="VU5" s="0"/>
+      <c r="VV5" s="0"/>
+      <c r="VW5" s="0"/>
+      <c r="VX5" s="0"/>
+      <c r="VY5" s="0"/>
+      <c r="VZ5" s="0"/>
+      <c r="WA5" s="0"/>
+      <c r="WB5" s="0"/>
+      <c r="WC5" s="0"/>
+      <c r="WD5" s="0"/>
+      <c r="WE5" s="0"/>
+      <c r="WF5" s="0"/>
+      <c r="WG5" s="0"/>
+      <c r="WH5" s="0"/>
+      <c r="WI5" s="0"/>
+      <c r="WJ5" s="0"/>
+      <c r="WK5" s="0"/>
+      <c r="WL5" s="0"/>
+      <c r="WM5" s="0"/>
+      <c r="WN5" s="0"/>
+      <c r="WO5" s="0"/>
+      <c r="WP5" s="0"/>
+      <c r="WQ5" s="0"/>
+      <c r="WR5" s="0"/>
+      <c r="WS5" s="0"/>
+      <c r="WT5" s="0"/>
+      <c r="WU5" s="0"/>
+      <c r="WV5" s="0"/>
+      <c r="WW5" s="0"/>
+      <c r="WX5" s="0"/>
+      <c r="WY5" s="0"/>
+      <c r="WZ5" s="0"/>
+      <c r="XA5" s="0"/>
+      <c r="XB5" s="0"/>
+      <c r="XC5" s="0"/>
+      <c r="XD5" s="0"/>
+      <c r="XE5" s="0"/>
+      <c r="XF5" s="0"/>
+      <c r="XG5" s="0"/>
+      <c r="XH5" s="0"/>
+      <c r="XI5" s="0"/>
+      <c r="XJ5" s="0"/>
+      <c r="XK5" s="0"/>
+      <c r="XL5" s="0"/>
+      <c r="XM5" s="0"/>
+      <c r="XN5" s="0"/>
+      <c r="XO5" s="0"/>
+      <c r="XP5" s="0"/>
+      <c r="XQ5" s="0"/>
+      <c r="XR5" s="0"/>
+      <c r="XS5" s="0"/>
+      <c r="XT5" s="0"/>
+      <c r="XU5" s="0"/>
+      <c r="XV5" s="0"/>
+      <c r="XW5" s="0"/>
+      <c r="XX5" s="0"/>
+      <c r="XY5" s="0"/>
+      <c r="XZ5" s="0"/>
+      <c r="YA5" s="0"/>
+      <c r="YB5" s="0"/>
+      <c r="YC5" s="0"/>
+      <c r="YD5" s="0"/>
+      <c r="YE5" s="0"/>
+      <c r="YF5" s="0"/>
+      <c r="YG5" s="0"/>
+      <c r="YH5" s="0"/>
+      <c r="YI5" s="0"/>
+      <c r="YJ5" s="0"/>
+      <c r="YK5" s="0"/>
+      <c r="YL5" s="0"/>
+      <c r="YM5" s="0"/>
+      <c r="YN5" s="0"/>
+      <c r="YO5" s="0"/>
+      <c r="YP5" s="0"/>
+      <c r="YQ5" s="0"/>
+      <c r="YR5" s="0"/>
+      <c r="YS5" s="0"/>
+      <c r="YT5" s="0"/>
+      <c r="YU5" s="0"/>
+      <c r="YV5" s="0"/>
+      <c r="YW5" s="0"/>
+      <c r="YX5" s="0"/>
+      <c r="YY5" s="0"/>
+      <c r="YZ5" s="0"/>
+      <c r="ZA5" s="0"/>
+      <c r="ZB5" s="0"/>
+      <c r="ZC5" s="0"/>
+      <c r="ZD5" s="0"/>
+      <c r="ZE5" s="0"/>
+      <c r="ZF5" s="0"/>
+      <c r="ZG5" s="0"/>
+      <c r="ZH5" s="0"/>
+      <c r="ZI5" s="0"/>
+      <c r="ZJ5" s="0"/>
+      <c r="ZK5" s="0"/>
+      <c r="ZL5" s="0"/>
+      <c r="ZM5" s="0"/>
+      <c r="ZN5" s="0"/>
+      <c r="ZO5" s="0"/>
+      <c r="ZP5" s="0"/>
+      <c r="ZQ5" s="0"/>
+      <c r="ZR5" s="0"/>
+      <c r="ZS5" s="0"/>
+      <c r="ZT5" s="0"/>
+      <c r="ZU5" s="0"/>
+      <c r="ZV5" s="0"/>
+      <c r="ZW5" s="0"/>
+      <c r="ZX5" s="0"/>
+      <c r="ZY5" s="0"/>
+      <c r="ZZ5" s="0"/>
+      <c r="AAA5" s="0"/>
+      <c r="AAB5" s="0"/>
+      <c r="AAC5" s="0"/>
+      <c r="AAD5" s="0"/>
+      <c r="AAE5" s="0"/>
+      <c r="AAF5" s="0"/>
+      <c r="AAG5" s="0"/>
+      <c r="AAH5" s="0"/>
+      <c r="AAI5" s="0"/>
+      <c r="AAJ5" s="0"/>
+      <c r="AAK5" s="0"/>
+      <c r="AAL5" s="0"/>
+      <c r="AAM5" s="0"/>
+      <c r="AAN5" s="0"/>
+      <c r="AAO5" s="0"/>
+      <c r="AAP5" s="0"/>
+      <c r="AAQ5" s="0"/>
+      <c r="AAR5" s="0"/>
+      <c r="AAS5" s="0"/>
+      <c r="AAT5" s="0"/>
+      <c r="AAU5" s="0"/>
+      <c r="AAV5" s="0"/>
+      <c r="AAW5" s="0"/>
+      <c r="AAX5" s="0"/>
+      <c r="AAY5" s="0"/>
+      <c r="AAZ5" s="0"/>
+      <c r="ABA5" s="0"/>
+      <c r="ABB5" s="0"/>
+      <c r="ABC5" s="0"/>
+      <c r="ABD5" s="0"/>
+      <c r="ABE5" s="0"/>
+      <c r="ABF5" s="0"/>
+      <c r="ABG5" s="0"/>
+      <c r="ABH5" s="0"/>
+      <c r="ABI5" s="0"/>
+      <c r="ABJ5" s="0"/>
+      <c r="ABK5" s="0"/>
+      <c r="ABL5" s="0"/>
+      <c r="ABM5" s="0"/>
+      <c r="ABN5" s="0"/>
+      <c r="ABO5" s="0"/>
+      <c r="ABP5" s="0"/>
+      <c r="ABQ5" s="0"/>
+      <c r="ABR5" s="0"/>
+      <c r="ABS5" s="0"/>
+      <c r="ABT5" s="0"/>
+      <c r="ABU5" s="0"/>
+      <c r="ABV5" s="0"/>
+      <c r="ABW5" s="0"/>
+      <c r="ABX5" s="0"/>
+      <c r="ABY5" s="0"/>
+      <c r="ABZ5" s="0"/>
+      <c r="ACA5" s="0"/>
+      <c r="ACB5" s="0"/>
+      <c r="ACC5" s="0"/>
+      <c r="ACD5" s="0"/>
+      <c r="ACE5" s="0"/>
+      <c r="ACF5" s="0"/>
+      <c r="ACG5" s="0"/>
+      <c r="ACH5" s="0"/>
+      <c r="ACI5" s="0"/>
+      <c r="ACJ5" s="0"/>
+      <c r="ACK5" s="0"/>
+      <c r="ACL5" s="0"/>
+      <c r="ACM5" s="0"/>
+      <c r="ACN5" s="0"/>
+      <c r="ACO5" s="0"/>
+      <c r="ACP5" s="0"/>
+      <c r="ACQ5" s="0"/>
+      <c r="ACR5" s="0"/>
+      <c r="ACS5" s="0"/>
+      <c r="ACT5" s="0"/>
+      <c r="ACU5" s="0"/>
+      <c r="ACV5" s="0"/>
+      <c r="ACW5" s="0"/>
+      <c r="ACX5" s="0"/>
+      <c r="ACY5" s="0"/>
+      <c r="ACZ5" s="0"/>
+      <c r="ADA5" s="0"/>
+      <c r="ADB5" s="0"/>
+      <c r="ADC5" s="0"/>
+      <c r="ADD5" s="0"/>
+      <c r="ADE5" s="0"/>
+      <c r="ADF5" s="0"/>
+      <c r="ADG5" s="0"/>
+      <c r="ADH5" s="0"/>
+      <c r="ADI5" s="0"/>
+      <c r="ADJ5" s="0"/>
+      <c r="ADK5" s="0"/>
+      <c r="ADL5" s="0"/>
+      <c r="ADM5" s="0"/>
+      <c r="ADN5" s="0"/>
+      <c r="ADO5" s="0"/>
+      <c r="ADP5" s="0"/>
+      <c r="ADQ5" s="0"/>
+      <c r="ADR5" s="0"/>
+      <c r="ADS5" s="0"/>
+      <c r="ADT5" s="0"/>
+      <c r="ADU5" s="0"/>
+      <c r="ADV5" s="0"/>
+      <c r="ADW5" s="0"/>
+      <c r="ADX5" s="0"/>
+      <c r="ADY5" s="0"/>
+      <c r="ADZ5" s="0"/>
+      <c r="AEA5" s="0"/>
+      <c r="AEB5" s="0"/>
+      <c r="AEC5" s="0"/>
+      <c r="AED5" s="0"/>
+      <c r="AEE5" s="0"/>
+      <c r="AEF5" s="0"/>
+      <c r="AEG5" s="0"/>
+      <c r="AEH5" s="0"/>
+      <c r="AEI5" s="0"/>
+      <c r="AEJ5" s="0"/>
+      <c r="AEK5" s="0"/>
+      <c r="AEL5" s="0"/>
+      <c r="AEM5" s="0"/>
+      <c r="AEN5" s="0"/>
+      <c r="AEO5" s="0"/>
+      <c r="AEP5" s="0"/>
+      <c r="AEQ5" s="0"/>
+      <c r="AER5" s="0"/>
+      <c r="AES5" s="0"/>
+      <c r="AET5" s="0"/>
+      <c r="AEU5" s="0"/>
+      <c r="AEV5" s="0"/>
+      <c r="AEW5" s="0"/>
+      <c r="AEX5" s="0"/>
+      <c r="AEY5" s="0"/>
+      <c r="AEZ5" s="0"/>
+      <c r="AFA5" s="0"/>
+      <c r="AFB5" s="0"/>
+      <c r="AFC5" s="0"/>
+      <c r="AFD5" s="0"/>
+      <c r="AFE5" s="0"/>
+      <c r="AFF5" s="0"/>
+      <c r="AFG5" s="0"/>
+      <c r="AFH5" s="0"/>
+      <c r="AFI5" s="0"/>
+      <c r="AFJ5" s="0"/>
+      <c r="AFK5" s="0"/>
+      <c r="AFL5" s="0"/>
+      <c r="AFM5" s="0"/>
+      <c r="AFN5" s="0"/>
+      <c r="AFO5" s="0"/>
+      <c r="AFP5" s="0"/>
+      <c r="AFQ5" s="0"/>
+      <c r="AFR5" s="0"/>
+      <c r="AFS5" s="0"/>
+      <c r="AFT5" s="0"/>
+      <c r="AFU5" s="0"/>
+      <c r="AFV5" s="0"/>
+      <c r="AFW5" s="0"/>
+      <c r="AFX5" s="0"/>
+      <c r="AFY5" s="0"/>
+      <c r="AFZ5" s="0"/>
+      <c r="AGA5" s="0"/>
+      <c r="AGB5" s="0"/>
+      <c r="AGC5" s="0"/>
+      <c r="AGD5" s="0"/>
+      <c r="AGE5" s="0"/>
+      <c r="AGF5" s="0"/>
+      <c r="AGG5" s="0"/>
+      <c r="AGH5" s="0"/>
+      <c r="AGI5" s="0"/>
+      <c r="AGJ5" s="0"/>
+      <c r="AGK5" s="0"/>
+      <c r="AGL5" s="0"/>
+      <c r="AGM5" s="0"/>
+      <c r="AGN5" s="0"/>
+      <c r="AGO5" s="0"/>
+      <c r="AGP5" s="0"/>
+      <c r="AGQ5" s="0"/>
+      <c r="AGR5" s="0"/>
+      <c r="AGS5" s="0"/>
+      <c r="AGT5" s="0"/>
+      <c r="AGU5" s="0"/>
+      <c r="AGV5" s="0"/>
+      <c r="AGW5" s="0"/>
+      <c r="AGX5" s="0"/>
+      <c r="AGY5" s="0"/>
+      <c r="AGZ5" s="0"/>
+      <c r="AHA5" s="0"/>
+      <c r="AHB5" s="0"/>
+      <c r="AHC5" s="0"/>
+      <c r="AHD5" s="0"/>
+      <c r="AHE5" s="0"/>
+      <c r="AHF5" s="0"/>
+      <c r="AHG5" s="0"/>
+      <c r="AHH5" s="0"/>
+      <c r="AHI5" s="0"/>
+      <c r="AHJ5" s="0"/>
+      <c r="AHK5" s="0"/>
+      <c r="AHL5" s="0"/>
+      <c r="AHM5" s="0"/>
+      <c r="AHN5" s="0"/>
+      <c r="AHO5" s="0"/>
+      <c r="AHP5" s="0"/>
+      <c r="AHQ5" s="0"/>
+      <c r="AHR5" s="0"/>
+      <c r="AHS5" s="0"/>
+      <c r="AHT5" s="0"/>
+      <c r="AHU5" s="0"/>
+      <c r="AHV5" s="0"/>
+      <c r="AHW5" s="0"/>
+      <c r="AHX5" s="0"/>
+      <c r="AHY5" s="0"/>
+      <c r="AHZ5" s="0"/>
+      <c r="AIA5" s="0"/>
+      <c r="AIB5" s="0"/>
+      <c r="AIC5" s="0"/>
+      <c r="AID5" s="0"/>
+      <c r="AIE5" s="0"/>
+      <c r="AIF5" s="0"/>
+      <c r="AIG5" s="0"/>
+      <c r="AIH5" s="0"/>
+      <c r="AII5" s="0"/>
+      <c r="AIJ5" s="0"/>
+      <c r="AIK5" s="0"/>
+      <c r="AIL5" s="0"/>
+      <c r="AIM5" s="0"/>
+      <c r="AIN5" s="0"/>
+      <c r="AIO5" s="0"/>
+      <c r="AIP5" s="0"/>
+      <c r="AIQ5" s="0"/>
+      <c r="AIR5" s="0"/>
+      <c r="AIS5" s="0"/>
+      <c r="AIT5" s="0"/>
+      <c r="AIU5" s="0"/>
+      <c r="AIV5" s="0"/>
+      <c r="AIW5" s="0"/>
+      <c r="AIX5" s="0"/>
+      <c r="AIY5" s="0"/>
+      <c r="AIZ5" s="0"/>
+      <c r="AJA5" s="0"/>
+      <c r="AJB5" s="0"/>
+      <c r="AJC5" s="0"/>
+      <c r="AJD5" s="0"/>
+      <c r="AJE5" s="0"/>
+      <c r="AJF5" s="0"/>
+      <c r="AJG5" s="0"/>
+      <c r="AJH5" s="0"/>
+      <c r="AJI5" s="0"/>
+      <c r="AJJ5" s="0"/>
+      <c r="AJK5" s="0"/>
+      <c r="AJL5" s="0"/>
+      <c r="AJM5" s="0"/>
+      <c r="AJN5" s="0"/>
+      <c r="AJO5" s="0"/>
+      <c r="AJP5" s="0"/>
+      <c r="AJQ5" s="0"/>
+      <c r="AJR5" s="0"/>
+      <c r="AJS5" s="0"/>
+      <c r="AJT5" s="0"/>
+      <c r="AJU5" s="0"/>
+      <c r="AJV5" s="0"/>
+      <c r="AJW5" s="0"/>
+      <c r="AJX5" s="0"/>
+      <c r="AJY5" s="0"/>
+      <c r="AJZ5" s="0"/>
+      <c r="AKA5" s="0"/>
+      <c r="AKB5" s="0"/>
+      <c r="AKC5" s="0"/>
+      <c r="AKD5" s="0"/>
+      <c r="AKE5" s="0"/>
+      <c r="AKF5" s="0"/>
+      <c r="AKG5" s="0"/>
+      <c r="AKH5" s="0"/>
+      <c r="AKI5" s="0"/>
+      <c r="AKJ5" s="0"/>
+      <c r="AKK5" s="0"/>
+      <c r="AKL5" s="0"/>
+      <c r="AKM5" s="0"/>
+      <c r="AKN5" s="0"/>
+      <c r="AKO5" s="0"/>
+      <c r="AKP5" s="0"/>
+      <c r="AKQ5" s="0"/>
+      <c r="AKR5" s="0"/>
+      <c r="AKS5" s="0"/>
+      <c r="AKT5" s="0"/>
+      <c r="AKU5" s="0"/>
+      <c r="AKV5" s="0"/>
+      <c r="AKW5" s="0"/>
+      <c r="AKX5" s="0"/>
+      <c r="AKY5" s="0"/>
+      <c r="AKZ5" s="0"/>
+      <c r="ALA5" s="0"/>
+      <c r="ALB5" s="0"/>
+      <c r="ALC5" s="0"/>
+      <c r="ALD5" s="0"/>
+      <c r="ALE5" s="0"/>
+      <c r="ALF5" s="0"/>
+      <c r="ALG5" s="0"/>
+      <c r="ALH5" s="0"/>
+      <c r="ALI5" s="0"/>
+      <c r="ALJ5" s="0"/>
+      <c r="ALK5" s="0"/>
+      <c r="ALL5" s="0"/>
+      <c r="ALM5" s="0"/>
+      <c r="ALN5" s="0"/>
+      <c r="ALO5" s="0"/>
+      <c r="ALP5" s="0"/>
+      <c r="ALQ5" s="0"/>
+      <c r="ALR5" s="0"/>
+      <c r="ALS5" s="0"/>
+      <c r="ALT5" s="0"/>
+      <c r="ALU5" s="0"/>
+      <c r="ALV5" s="0"/>
+      <c r="ALW5" s="0"/>
+      <c r="ALX5" s="0"/>
+      <c r="ALY5" s="0"/>
+      <c r="ALZ5" s="0"/>
+      <c r="AMA5" s="0"/>
+      <c r="AMB5" s="0"/>
+      <c r="AMC5" s="0"/>
+      <c r="AMD5" s="0"/>
+      <c r="AME5" s="0"/>
+      <c r="AMF5" s="0"/>
+      <c r="AMG5" s="0"/>
+      <c r="AMH5" s="0"/>
+      <c r="AMI5" s="0"/>
+      <c r="AMJ5" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -346,13 +1362,13 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.74"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="11.52"/>
   </cols>
@@ -400,7 +1416,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -447,7 +1463,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -474,7 +1490,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
regressregression of infrastructure spending on age of housing stock
</commit_message>
<xml_diff>
--- a/reference/20220805 Data Dictionary.xlsx
+++ b/reference/20220805 Data Dictionary.xlsx
@@ -69,10 +69,11 @@
     <t xml:space="preserve">Block Group Housing (2013).Rds</t>
   </si>
   <si>
-    <t xml:space="preserve">Median year built and total number of housing units by census block group.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compiled from the 2013 vintage of the American Community Survey.</t>
+    <t xml:space="preserve">Median year built and total number of housing units at both the Census block group and county level.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compiled from the 2013 vintage of the American Community Survey. 
+Note that block groups generally contain 600–3,000 people, and never cross state, county, or census tract boundaries.</t>
   </si>
   <si>
     <t xml:space="preserve">Field</t>
@@ -261,11 +262,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -301,7 +302,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="71.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="85.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="96.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="11.57"/>
   </cols>
@@ -362,14 +363,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="3" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -416,10 +417,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -430,10 +431,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="6" t="s">

</xml_diff>